<commit_message>
update daily for ck and crypto
</commit_message>
<xml_diff>
--- a/trade_log.xlsx
+++ b/trade_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\working\trading\binance_cron\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56A4233C-CB5E-4F04-BDC7-8858C7F4B41F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35DE0640-4CD2-4104-B1E8-0922B4424DE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
   <si>
     <t>STT</t>
   </si>
@@ -54,9 +54,6 @@
     <t>Giá Thoát</t>
   </si>
   <si>
-    <t>Số lượng</t>
-  </si>
-  <si>
     <t>Lợi Nhuận</t>
   </si>
   <si>
@@ -72,9 +69,6 @@
     <t>BTC/USDT</t>
   </si>
   <si>
-    <t>mua khi macd âm, ema âm</t>
-  </si>
-  <si>
     <t>6/12/2025</t>
   </si>
   <si>
@@ -109,13 +103,31 @@
   </si>
   <si>
     <t xml:space="preserve">Tổng lợi nhuận  </t>
+  </si>
+  <si>
+    <t>17/12/2025</t>
+  </si>
+  <si>
+    <t>mua</t>
+  </si>
+  <si>
+    <t xml:space="preserve">btc/usdt </t>
+  </si>
+  <si>
+    <t>kích thước</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bắt đáy , sai quy tắc vào lệnh </t>
+  </si>
+  <si>
+    <t>bán khi macd âm, ema âm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,6 +144,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -172,12 +191,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -483,7 +503,7 @@
   <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -515,13 +535,13 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -529,13 +549,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
       </c>
       <c r="E2">
         <v>90800</v>
@@ -550,65 +570,65 @@
         <v>12.34</v>
       </c>
       <c r="J2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="D3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="3">
+        <v>13.819000000000001</v>
+      </c>
+      <c r="G3" s="3">
+        <v>13.974</v>
+      </c>
+      <c r="H3" s="3">
+        <v>4.82</v>
+      </c>
+      <c r="I3" s="3">
+        <v>0.74</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" t="s">
+    <row r="4" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E3">
-        <v>13.819000000000001</v>
-      </c>
-      <c r="G3">
-        <v>13.974</v>
-      </c>
-      <c r="H3">
-        <v>4.82</v>
-      </c>
-      <c r="I3">
-        <v>0.74</v>
-      </c>
-      <c r="J3" t="s">
+      <c r="C4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="E4" s="3">
+        <v>910.61</v>
+      </c>
+      <c r="G4" s="3">
+        <v>902.2</v>
+      </c>
+      <c r="H4" s="3">
+        <v>0.22</v>
+      </c>
+      <c r="I4" s="3">
+        <v>-1.85</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4">
-        <v>910.61</v>
-      </c>
-      <c r="G4">
-        <v>902.2</v>
-      </c>
-      <c r="H4">
-        <v>0.22</v>
-      </c>
-      <c r="I4">
-        <v>-1.85</v>
-      </c>
-      <c r="J4" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -616,13 +636,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E5">
         <v>193.96</v>
@@ -640,44 +660,70 @@
         <v>4.62</v>
       </c>
       <c r="J5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6">
+    <row r="6" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="B6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="3">
+        <v>199.4</v>
+      </c>
+      <c r="F6" s="3">
+        <v>196</v>
+      </c>
+      <c r="G6" s="3">
+        <v>198.5</v>
+      </c>
+      <c r="H6" s="3">
+        <v>0.33900000000000002</v>
+      </c>
+      <c r="I6" s="3">
+        <v>-1.6</v>
+      </c>
+      <c r="J6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E6">
-        <v>199.4</v>
-      </c>
-      <c r="F6">
-        <v>196</v>
-      </c>
-      <c r="G6">
-        <v>198.5</v>
-      </c>
-      <c r="H6">
-        <v>0.33900000000000002</v>
-      </c>
-      <c r="I6">
-        <v>-1.6</v>
-      </c>
-      <c r="J6" t="s">
+    </row>
+    <row r="7" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>24</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="3">
+        <v>88098</v>
+      </c>
+      <c r="F7" s="3">
+        <v>85000</v>
+      </c>
+      <c r="H7" s="3">
+        <v>261</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H21" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="I21" s="2">
         <f xml:space="preserve"> SUM(I2:I20)</f>

</xml_diff>